<commit_message>
Semi updated BinaAz service.
</commit_message>
<xml_diff>
--- a/DatabaseColumns.xlsx
+++ b/DatabaseColumns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -24,6 +24,9 @@
     <t>bigint</t>
   </si>
   <si>
+    <t>+</t>
+  </si>
+  <si>
     <t>address</t>
   </si>
   <si>
@@ -51,22 +54,43 @@
     <t>X</t>
   </si>
   <si>
+    <t>metaTags</t>
+  </si>
+  <si>
+    <t>titlecontent</t>
+  </si>
+  <si>
     <t>area</t>
   </si>
   <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearest Locations</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
     <t>binatype</t>
   </si>
   <si>
     <t>torpaqarea</t>
   </si>
   <si>
+    <t>landArea</t>
+  </si>
+  <si>
     <t>category</t>
   </si>
   <si>
     <t>nvarchar(35)</t>
   </si>
   <si>
-    <t>+</t>
+    <t>price</t>
   </si>
   <si>
     <t>[document]</t>
@@ -84,12 +108,21 @@
     <t>renovation</t>
   </si>
   <si>
+    <t>hasRepair</t>
+  </si>
+  <si>
     <t>insertdate</t>
   </si>
   <si>
+    <t>hasBillOfSale</t>
+  </si>
+  <si>
     <t>ipoteka</t>
   </si>
   <si>
+    <t>hasMortgage</t>
+  </si>
+  <si>
     <t>item_id</t>
   </si>
   <si>
@@ -105,12 +138,18 @@
     <t>room</t>
   </si>
   <si>
+    <t>rooms</t>
+  </si>
+  <si>
     <t>poster_note</t>
   </si>
   <si>
     <t>post_tip</t>
   </si>
   <si>
+    <t>id|name</t>
+  </si>
+  <si>
     <t>poster_type</t>
   </si>
   <si>
@@ -123,6 +162,18 @@
     <t>-</t>
   </si>
   <si>
+    <t>contactName</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>leased</t>
+  </si>
+  <si>
+    <t>contactTypeName</t>
+  </si>
+  <si>
     <t>updated</t>
   </si>
   <si>
@@ -136,6 +187,12 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>homepage</t>
   </si>
   <si>
     <t>sayt_link</t>
@@ -173,8 +230,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,6 +744,10 @@
     <col bestFit="1" min="4" max="4" width="15.7109375"/>
     <col bestFit="1" min="5" max="5" width="13.57421875"/>
     <col bestFit="1" customWidth="1" min="6" max="6" width="13.57421875"/>
+    <col bestFit="1" min="11" max="11" width="15.7109375"/>
+    <col bestFit="1" min="13" max="13" width="4.00390625"/>
+    <col bestFit="1" min="14" max="14" width="15.8515625"/>
+    <col bestFit="1" min="15" max="15" width="7.57421875"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.25">
@@ -703,551 +767,791 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(E2=F2,"T","F")</f>
+        <f t="shared" ref="G2:G9" si="0">IF(E2=F2,"T","F")</f>
         <v>T</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="str">
-        <f>IF(E3=F3,"T","F")</f>
-        <v>T</v>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="str">
-        <f>IF(E4=F4,"T","F")</f>
-        <v>F</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
+      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" t="str">
-        <f>IF(E5=F5,"T","F")</f>
-        <v>T</v>
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(E6=F6,"T","F")</f>
+        <f t="shared" si="0"/>
         <v>T</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" t="str">
-        <f>IF(E7=F7,"T","F")</f>
+        <f t="shared" si="0"/>
         <v>T</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="str">
-        <f>IF(E8=F8,"T","F")</f>
-        <v>F</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G9" t="str">
-        <f>IF(E9=F9,"T","F")</f>
+        <f t="shared" si="0"/>
         <v>F</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" t="str">
-        <f>IF(E10=F10,"T","F")</f>
+        <f t="shared" ref="G10:G27" si="1">IF(E10=F10,"T","F")</f>
         <v>F</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" t="str">
-        <f>IF(E11=F11,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" t="str">
-        <f>IF(E12=F12,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G13" t="str">
-        <f>IF(E13=F13,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G14" t="str">
-        <f>IF(E14=F14,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15" t="str">
-        <f>IF(E15=F15,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" t="str">
-        <f>IF(E16=F16,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17" t="str">
-        <f>IF(E17=F17,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G18" t="str">
-        <f>IF(E18=F18,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G19" t="str">
-        <f>IF(E19=F19,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20" t="str">
-        <f>IF(E20=F20,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" t="str">
-        <f>IF(E21=F21,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G22" t="str">
-        <f>IF(E22=F22,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L22" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G23" t="str">
-        <f>IF(E23=F23,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H23" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G24" t="str">
-        <f>IF(E24=F24,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H24" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="25" ht="14.25">
       <c r="D25" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G25" t="str">
-        <f>IF(E25=F25,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>F</v>
       </c>
       <c r="H25" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="D26" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G26" t="str">
-        <f>IF(E26=F26,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="D27" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G27" t="str">
-        <f>IF(E27=F27,"T","F")</f>
+        <f t="shared" si="1"/>
         <v>T</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>